<commit_message>
Refactor Argument Parser Usage
</commit_message>
<xml_diff>
--- a/default_report_template.xlsx
+++ b/default_report_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AVAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F39BBF8-F5BC-4465-9471-26781A1B323E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64810AD2-03EE-4DC8-AC99-2325F46CD6FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18750" yWindow="1920" windowWidth="21825" windowHeight="15435" tabRatio="923" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" tabRatio="923" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="표지" sheetId="148" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2985" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2989" uniqueCount="109">
   <si>
     <t>구분</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1379,6 +1379,15 @@
     <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1451,6 +1460,15 @@
     <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1465,6 +1483,9 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1657,27 +1678,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3946,13 +3946,13 @@
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
       <c r="AR1" s="1"/>
-      <c r="AS1" s="24" t="s">
+      <c r="AS1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="AT1" s="25"/>
-      <c r="AU1" s="25"/>
-      <c r="AV1" s="25"/>
-      <c r="AW1" s="26"/>
+      <c r="AT1" s="28"/>
+      <c r="AU1" s="28"/>
+      <c r="AV1" s="28"/>
+      <c r="AW1" s="29"/>
       <c r="AX1" s="1"/>
     </row>
     <row r="2" spans="1:50" x14ac:dyDescent="0.3">
@@ -3962,18 +3962,18 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="33" t="s">
+      <c r="G2" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="35"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="38"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
@@ -4002,11 +4002,11 @@
       <c r="AP2" s="1"/>
       <c r="AQ2" s="1"/>
       <c r="AR2" s="1"/>
-      <c r="AS2" s="27"/>
-      <c r="AT2" s="28"/>
-      <c r="AU2" s="28"/>
-      <c r="AV2" s="28"/>
-      <c r="AW2" s="29"/>
+      <c r="AS2" s="30"/>
+      <c r="AT2" s="31"/>
+      <c r="AU2" s="31"/>
+      <c r="AV2" s="31"/>
+      <c r="AW2" s="32"/>
       <c r="AX2" s="1"/>
     </row>
     <row r="3" spans="1:50" ht="14.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -4016,16 +4016,16 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="38"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="41"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -4053,11 +4053,11 @@
       <c r="AP3" s="1"/>
       <c r="AQ3" s="1"/>
       <c r="AR3" s="1"/>
-      <c r="AS3" s="30"/>
-      <c r="AT3" s="31"/>
-      <c r="AU3" s="31"/>
-      <c r="AV3" s="31"/>
-      <c r="AW3" s="32"/>
+      <c r="AS3" s="33"/>
+      <c r="AT3" s="34"/>
+      <c r="AU3" s="34"/>
+      <c r="AV3" s="34"/>
+      <c r="AW3" s="35"/>
       <c r="AX3" s="1"/>
     </row>
     <row r="4" spans="1:50" x14ac:dyDescent="0.3">
@@ -4067,16 +4067,16 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
-      <c r="N4" s="40"/>
-      <c r="O4" s="40"/>
-      <c r="P4" s="41"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="43"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="44"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
@@ -4424,38 +4424,38 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-      <c r="K11" s="42" t="s">
+      <c r="K11" s="45" t="s">
         <v>101</v>
       </c>
-      <c r="L11" s="43"/>
-      <c r="M11" s="43"/>
-      <c r="N11" s="43"/>
-      <c r="O11" s="43"/>
-      <c r="P11" s="43"/>
-      <c r="Q11" s="43"/>
-      <c r="R11" s="43"/>
-      <c r="S11" s="43"/>
-      <c r="T11" s="43"/>
-      <c r="U11" s="43"/>
-      <c r="V11" s="43"/>
-      <c r="W11" s="43"/>
-      <c r="X11" s="43"/>
-      <c r="Y11" s="43"/>
-      <c r="Z11" s="43"/>
-      <c r="AA11" s="43"/>
-      <c r="AB11" s="43"/>
-      <c r="AC11" s="43"/>
-      <c r="AD11" s="43"/>
-      <c r="AE11" s="43"/>
-      <c r="AF11" s="43"/>
-      <c r="AG11" s="43"/>
-      <c r="AH11" s="43"/>
-      <c r="AI11" s="43"/>
-      <c r="AJ11" s="43"/>
-      <c r="AK11" s="43"/>
-      <c r="AL11" s="43"/>
-      <c r="AM11" s="43"/>
-      <c r="AN11" s="43"/>
+      <c r="L11" s="46"/>
+      <c r="M11" s="46"/>
+      <c r="N11" s="46"/>
+      <c r="O11" s="46"/>
+      <c r="P11" s="46"/>
+      <c r="Q11" s="46"/>
+      <c r="R11" s="46"/>
+      <c r="S11" s="46"/>
+      <c r="T11" s="46"/>
+      <c r="U11" s="46"/>
+      <c r="V11" s="46"/>
+      <c r="W11" s="46"/>
+      <c r="X11" s="46"/>
+      <c r="Y11" s="46"/>
+      <c r="Z11" s="46"/>
+      <c r="AA11" s="46"/>
+      <c r="AB11" s="46"/>
+      <c r="AC11" s="46"/>
+      <c r="AD11" s="46"/>
+      <c r="AE11" s="46"/>
+      <c r="AF11" s="46"/>
+      <c r="AG11" s="46"/>
+      <c r="AH11" s="46"/>
+      <c r="AI11" s="46"/>
+      <c r="AJ11" s="46"/>
+      <c r="AK11" s="46"/>
+      <c r="AL11" s="46"/>
+      <c r="AM11" s="46"/>
+      <c r="AN11" s="46"/>
       <c r="AO11" s="1"/>
       <c r="AP11" s="1"/>
       <c r="AQ11" s="1"/>
@@ -4478,36 +4478,36 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="44"/>
-      <c r="L12" s="44"/>
-      <c r="M12" s="44"/>
-      <c r="N12" s="44"/>
-      <c r="O12" s="44"/>
-      <c r="P12" s="44"/>
-      <c r="Q12" s="44"/>
-      <c r="R12" s="44"/>
-      <c r="S12" s="44"/>
-      <c r="T12" s="44"/>
-      <c r="U12" s="44"/>
-      <c r="V12" s="44"/>
-      <c r="W12" s="44"/>
-      <c r="X12" s="44"/>
-      <c r="Y12" s="44"/>
-      <c r="Z12" s="44"/>
-      <c r="AA12" s="44"/>
-      <c r="AB12" s="44"/>
-      <c r="AC12" s="44"/>
-      <c r="AD12" s="44"/>
-      <c r="AE12" s="44"/>
-      <c r="AF12" s="44"/>
-      <c r="AG12" s="44"/>
-      <c r="AH12" s="44"/>
-      <c r="AI12" s="44"/>
-      <c r="AJ12" s="44"/>
-      <c r="AK12" s="44"/>
-      <c r="AL12" s="44"/>
-      <c r="AM12" s="44"/>
-      <c r="AN12" s="44"/>
+      <c r="K12" s="47"/>
+      <c r="L12" s="47"/>
+      <c r="M12" s="47"/>
+      <c r="N12" s="47"/>
+      <c r="O12" s="47"/>
+      <c r="P12" s="47"/>
+      <c r="Q12" s="47"/>
+      <c r="R12" s="47"/>
+      <c r="S12" s="47"/>
+      <c r="T12" s="47"/>
+      <c r="U12" s="47"/>
+      <c r="V12" s="47"/>
+      <c r="W12" s="47"/>
+      <c r="X12" s="47"/>
+      <c r="Y12" s="47"/>
+      <c r="Z12" s="47"/>
+      <c r="AA12" s="47"/>
+      <c r="AB12" s="47"/>
+      <c r="AC12" s="47"/>
+      <c r="AD12" s="47"/>
+      <c r="AE12" s="47"/>
+      <c r="AF12" s="47"/>
+      <c r="AG12" s="47"/>
+      <c r="AH12" s="47"/>
+      <c r="AI12" s="47"/>
+      <c r="AJ12" s="47"/>
+      <c r="AK12" s="47"/>
+      <c r="AL12" s="47"/>
+      <c r="AM12" s="47"/>
+      <c r="AN12" s="47"/>
       <c r="AO12" s="1"/>
       <c r="AP12" s="1"/>
       <c r="AQ12" s="1"/>
@@ -4530,36 +4530,36 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
-      <c r="K13" s="44"/>
-      <c r="L13" s="44"/>
-      <c r="M13" s="44"/>
-      <c r="N13" s="44"/>
-      <c r="O13" s="44"/>
-      <c r="P13" s="44"/>
-      <c r="Q13" s="44"/>
-      <c r="R13" s="44"/>
-      <c r="S13" s="44"/>
-      <c r="T13" s="44"/>
-      <c r="U13" s="44"/>
-      <c r="V13" s="44"/>
-      <c r="W13" s="44"/>
-      <c r="X13" s="44"/>
-      <c r="Y13" s="44"/>
-      <c r="Z13" s="44"/>
-      <c r="AA13" s="44"/>
-      <c r="AB13" s="44"/>
-      <c r="AC13" s="44"/>
-      <c r="AD13" s="44"/>
-      <c r="AE13" s="44"/>
-      <c r="AF13" s="44"/>
-      <c r="AG13" s="44"/>
-      <c r="AH13" s="44"/>
-      <c r="AI13" s="44"/>
-      <c r="AJ13" s="44"/>
-      <c r="AK13" s="44"/>
-      <c r="AL13" s="44"/>
-      <c r="AM13" s="44"/>
-      <c r="AN13" s="44"/>
+      <c r="K13" s="47"/>
+      <c r="L13" s="47"/>
+      <c r="M13" s="47"/>
+      <c r="N13" s="47"/>
+      <c r="O13" s="47"/>
+      <c r="P13" s="47"/>
+      <c r="Q13" s="47"/>
+      <c r="R13" s="47"/>
+      <c r="S13" s="47"/>
+      <c r="T13" s="47"/>
+      <c r="U13" s="47"/>
+      <c r="V13" s="47"/>
+      <c r="W13" s="47"/>
+      <c r="X13" s="47"/>
+      <c r="Y13" s="47"/>
+      <c r="Z13" s="47"/>
+      <c r="AA13" s="47"/>
+      <c r="AB13" s="47"/>
+      <c r="AC13" s="47"/>
+      <c r="AD13" s="47"/>
+      <c r="AE13" s="47"/>
+      <c r="AF13" s="47"/>
+      <c r="AG13" s="47"/>
+      <c r="AH13" s="47"/>
+      <c r="AI13" s="47"/>
+      <c r="AJ13" s="47"/>
+      <c r="AK13" s="47"/>
+      <c r="AL13" s="47"/>
+      <c r="AM13" s="47"/>
+      <c r="AN13" s="47"/>
       <c r="AO13" s="1"/>
       <c r="AP13" s="1"/>
       <c r="AQ13" s="1"/>
@@ -4582,36 +4582,36 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
-      <c r="K14" s="44"/>
-      <c r="L14" s="44"/>
-      <c r="M14" s="44"/>
-      <c r="N14" s="44"/>
-      <c r="O14" s="44"/>
-      <c r="P14" s="44"/>
-      <c r="Q14" s="44"/>
-      <c r="R14" s="44"/>
-      <c r="S14" s="44"/>
-      <c r="T14" s="44"/>
-      <c r="U14" s="44"/>
-      <c r="V14" s="44"/>
-      <c r="W14" s="44"/>
-      <c r="X14" s="44"/>
-      <c r="Y14" s="44"/>
-      <c r="Z14" s="44"/>
-      <c r="AA14" s="44"/>
-      <c r="AB14" s="44"/>
-      <c r="AC14" s="44"/>
-      <c r="AD14" s="44"/>
-      <c r="AE14" s="44"/>
-      <c r="AF14" s="44"/>
-      <c r="AG14" s="44"/>
-      <c r="AH14" s="44"/>
-      <c r="AI14" s="44"/>
-      <c r="AJ14" s="44"/>
-      <c r="AK14" s="44"/>
-      <c r="AL14" s="44"/>
-      <c r="AM14" s="44"/>
-      <c r="AN14" s="44"/>
+      <c r="K14" s="47"/>
+      <c r="L14" s="47"/>
+      <c r="M14" s="47"/>
+      <c r="N14" s="47"/>
+      <c r="O14" s="47"/>
+      <c r="P14" s="47"/>
+      <c r="Q14" s="47"/>
+      <c r="R14" s="47"/>
+      <c r="S14" s="47"/>
+      <c r="T14" s="47"/>
+      <c r="U14" s="47"/>
+      <c r="V14" s="47"/>
+      <c r="W14" s="47"/>
+      <c r="X14" s="47"/>
+      <c r="Y14" s="47"/>
+      <c r="Z14" s="47"/>
+      <c r="AA14" s="47"/>
+      <c r="AB14" s="47"/>
+      <c r="AC14" s="47"/>
+      <c r="AD14" s="47"/>
+      <c r="AE14" s="47"/>
+      <c r="AF14" s="47"/>
+      <c r="AG14" s="47"/>
+      <c r="AH14" s="47"/>
+      <c r="AI14" s="47"/>
+      <c r="AJ14" s="47"/>
+      <c r="AK14" s="47"/>
+      <c r="AL14" s="47"/>
+      <c r="AM14" s="47"/>
+      <c r="AN14" s="47"/>
       <c r="AO14" s="1"/>
       <c r="AP14" s="1"/>
       <c r="AQ14" s="1"/>
@@ -4634,36 +4634,36 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
-      <c r="K15" s="44"/>
-      <c r="L15" s="44"/>
-      <c r="M15" s="44"/>
-      <c r="N15" s="44"/>
-      <c r="O15" s="44"/>
-      <c r="P15" s="44"/>
-      <c r="Q15" s="44"/>
-      <c r="R15" s="44"/>
-      <c r="S15" s="44"/>
-      <c r="T15" s="44"/>
-      <c r="U15" s="44"/>
-      <c r="V15" s="44"/>
-      <c r="W15" s="44"/>
-      <c r="X15" s="44"/>
-      <c r="Y15" s="44"/>
-      <c r="Z15" s="44"/>
-      <c r="AA15" s="44"/>
-      <c r="AB15" s="44"/>
-      <c r="AC15" s="44"/>
-      <c r="AD15" s="44"/>
-      <c r="AE15" s="44"/>
-      <c r="AF15" s="44"/>
-      <c r="AG15" s="44"/>
-      <c r="AH15" s="44"/>
-      <c r="AI15" s="44"/>
-      <c r="AJ15" s="44"/>
-      <c r="AK15" s="44"/>
-      <c r="AL15" s="44"/>
-      <c r="AM15" s="44"/>
-      <c r="AN15" s="44"/>
+      <c r="K15" s="47"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="47"/>
+      <c r="N15" s="47"/>
+      <c r="O15" s="47"/>
+      <c r="P15" s="47"/>
+      <c r="Q15" s="47"/>
+      <c r="R15" s="47"/>
+      <c r="S15" s="47"/>
+      <c r="T15" s="47"/>
+      <c r="U15" s="47"/>
+      <c r="V15" s="47"/>
+      <c r="W15" s="47"/>
+      <c r="X15" s="47"/>
+      <c r="Y15" s="47"/>
+      <c r="Z15" s="47"/>
+      <c r="AA15" s="47"/>
+      <c r="AB15" s="47"/>
+      <c r="AC15" s="47"/>
+      <c r="AD15" s="47"/>
+      <c r="AE15" s="47"/>
+      <c r="AF15" s="47"/>
+      <c r="AG15" s="47"/>
+      <c r="AH15" s="47"/>
+      <c r="AI15" s="47"/>
+      <c r="AJ15" s="47"/>
+      <c r="AK15" s="47"/>
+      <c r="AL15" s="47"/>
+      <c r="AM15" s="47"/>
+      <c r="AN15" s="47"/>
       <c r="AO15" s="1"/>
       <c r="AP15" s="1"/>
       <c r="AQ15" s="1"/>
@@ -4686,36 +4686,36 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
-      <c r="K16" s="45"/>
-      <c r="L16" s="45"/>
-      <c r="M16" s="45"/>
-      <c r="N16" s="45"/>
-      <c r="O16" s="45"/>
-      <c r="P16" s="45"/>
-      <c r="Q16" s="45"/>
-      <c r="R16" s="45"/>
-      <c r="S16" s="45"/>
-      <c r="T16" s="45"/>
-      <c r="U16" s="45"/>
-      <c r="V16" s="45"/>
-      <c r="W16" s="45"/>
-      <c r="X16" s="45"/>
-      <c r="Y16" s="45"/>
-      <c r="Z16" s="45"/>
-      <c r="AA16" s="45"/>
-      <c r="AB16" s="45"/>
-      <c r="AC16" s="45"/>
-      <c r="AD16" s="45"/>
-      <c r="AE16" s="45"/>
-      <c r="AF16" s="45"/>
-      <c r="AG16" s="45"/>
-      <c r="AH16" s="45"/>
-      <c r="AI16" s="45"/>
-      <c r="AJ16" s="45"/>
-      <c r="AK16" s="45"/>
-      <c r="AL16" s="45"/>
-      <c r="AM16" s="45"/>
-      <c r="AN16" s="45"/>
+      <c r="K16" s="48"/>
+      <c r="L16" s="48"/>
+      <c r="M16" s="48"/>
+      <c r="N16" s="48"/>
+      <c r="O16" s="48"/>
+      <c r="P16" s="48"/>
+      <c r="Q16" s="48"/>
+      <c r="R16" s="48"/>
+      <c r="S16" s="48"/>
+      <c r="T16" s="48"/>
+      <c r="U16" s="48"/>
+      <c r="V16" s="48"/>
+      <c r="W16" s="48"/>
+      <c r="X16" s="48"/>
+      <c r="Y16" s="48"/>
+      <c r="Z16" s="48"/>
+      <c r="AA16" s="48"/>
+      <c r="AB16" s="48"/>
+      <c r="AC16" s="48"/>
+      <c r="AD16" s="48"/>
+      <c r="AE16" s="48"/>
+      <c r="AF16" s="48"/>
+      <c r="AG16" s="48"/>
+      <c r="AH16" s="48"/>
+      <c r="AI16" s="48"/>
+      <c r="AJ16" s="48"/>
+      <c r="AK16" s="48"/>
+      <c r="AL16" s="48"/>
+      <c r="AM16" s="48"/>
+      <c r="AN16" s="48"/>
       <c r="AO16" s="1"/>
       <c r="AP16" s="1"/>
       <c r="AQ16" s="1"/>
@@ -5051,36 +5051,36 @@
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
-      <c r="L23" s="46">
+      <c r="L23" s="49">
         <v>43831</v>
       </c>
-      <c r="M23" s="46"/>
-      <c r="N23" s="46"/>
-      <c r="O23" s="46"/>
-      <c r="P23" s="46"/>
-      <c r="Q23" s="46"/>
-      <c r="R23" s="46"/>
-      <c r="S23" s="46"/>
-      <c r="T23" s="46"/>
-      <c r="U23" s="46"/>
-      <c r="V23" s="46"/>
-      <c r="W23" s="46"/>
-      <c r="X23" s="46"/>
-      <c r="Y23" s="46"/>
-      <c r="Z23" s="46"/>
-      <c r="AA23" s="46"/>
-      <c r="AB23" s="46"/>
-      <c r="AC23" s="46"/>
-      <c r="AD23" s="46"/>
-      <c r="AE23" s="46"/>
-      <c r="AF23" s="46"/>
-      <c r="AG23" s="46"/>
-      <c r="AH23" s="46"/>
-      <c r="AI23" s="46"/>
-      <c r="AJ23" s="46"/>
-      <c r="AK23" s="46"/>
-      <c r="AL23" s="46"/>
-      <c r="AM23" s="46"/>
+      <c r="M23" s="49"/>
+      <c r="N23" s="49"/>
+      <c r="O23" s="49"/>
+      <c r="P23" s="49"/>
+      <c r="Q23" s="49"/>
+      <c r="R23" s="49"/>
+      <c r="S23" s="49"/>
+      <c r="T23" s="49"/>
+      <c r="U23" s="49"/>
+      <c r="V23" s="49"/>
+      <c r="W23" s="49"/>
+      <c r="X23" s="49"/>
+      <c r="Y23" s="49"/>
+      <c r="Z23" s="49"/>
+      <c r="AA23" s="49"/>
+      <c r="AB23" s="49"/>
+      <c r="AC23" s="49"/>
+      <c r="AD23" s="49"/>
+      <c r="AE23" s="49"/>
+      <c r="AF23" s="49"/>
+      <c r="AG23" s="49"/>
+      <c r="AH23" s="49"/>
+      <c r="AI23" s="49"/>
+      <c r="AJ23" s="49"/>
+      <c r="AK23" s="49"/>
+      <c r="AL23" s="49"/>
+      <c r="AM23" s="49"/>
       <c r="AN23" s="1"/>
       <c r="AO23" s="1"/>
       <c r="AP23" s="1"/>
@@ -5105,34 +5105,34 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
-      <c r="L24" s="46"/>
-      <c r="M24" s="46"/>
-      <c r="N24" s="46"/>
-      <c r="O24" s="46"/>
-      <c r="P24" s="46"/>
-      <c r="Q24" s="46"/>
-      <c r="R24" s="46"/>
-      <c r="S24" s="46"/>
-      <c r="T24" s="46"/>
-      <c r="U24" s="46"/>
-      <c r="V24" s="46"/>
-      <c r="W24" s="46"/>
-      <c r="X24" s="46"/>
-      <c r="Y24" s="46"/>
-      <c r="Z24" s="46"/>
-      <c r="AA24" s="46"/>
-      <c r="AB24" s="46"/>
-      <c r="AC24" s="46"/>
-      <c r="AD24" s="46"/>
-      <c r="AE24" s="46"/>
-      <c r="AF24" s="46"/>
-      <c r="AG24" s="46"/>
-      <c r="AH24" s="46"/>
-      <c r="AI24" s="46"/>
-      <c r="AJ24" s="46"/>
-      <c r="AK24" s="46"/>
-      <c r="AL24" s="46"/>
-      <c r="AM24" s="46"/>
+      <c r="L24" s="49"/>
+      <c r="M24" s="49"/>
+      <c r="N24" s="49"/>
+      <c r="O24" s="49"/>
+      <c r="P24" s="49"/>
+      <c r="Q24" s="49"/>
+      <c r="R24" s="49"/>
+      <c r="S24" s="49"/>
+      <c r="T24" s="49"/>
+      <c r="U24" s="49"/>
+      <c r="V24" s="49"/>
+      <c r="W24" s="49"/>
+      <c r="X24" s="49"/>
+      <c r="Y24" s="49"/>
+      <c r="Z24" s="49"/>
+      <c r="AA24" s="49"/>
+      <c r="AB24" s="49"/>
+      <c r="AC24" s="49"/>
+      <c r="AD24" s="49"/>
+      <c r="AE24" s="49"/>
+      <c r="AF24" s="49"/>
+      <c r="AG24" s="49"/>
+      <c r="AH24" s="49"/>
+      <c r="AI24" s="49"/>
+      <c r="AJ24" s="49"/>
+      <c r="AK24" s="49"/>
+      <c r="AL24" s="49"/>
+      <c r="AM24" s="49"/>
       <c r="AN24" s="1"/>
       <c r="AO24" s="1"/>
       <c r="AP24" s="1"/>
@@ -5157,34 +5157,34 @@
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
-      <c r="L25" s="46"/>
-      <c r="M25" s="46"/>
-      <c r="N25" s="46"/>
-      <c r="O25" s="46"/>
-      <c r="P25" s="46"/>
-      <c r="Q25" s="46"/>
-      <c r="R25" s="46"/>
-      <c r="S25" s="46"/>
-      <c r="T25" s="46"/>
-      <c r="U25" s="46"/>
-      <c r="V25" s="46"/>
-      <c r="W25" s="46"/>
-      <c r="X25" s="46"/>
-      <c r="Y25" s="46"/>
-      <c r="Z25" s="46"/>
-      <c r="AA25" s="46"/>
-      <c r="AB25" s="46"/>
-      <c r="AC25" s="46"/>
-      <c r="AD25" s="46"/>
-      <c r="AE25" s="46"/>
-      <c r="AF25" s="46"/>
-      <c r="AG25" s="46"/>
-      <c r="AH25" s="46"/>
-      <c r="AI25" s="46"/>
-      <c r="AJ25" s="46"/>
-      <c r="AK25" s="46"/>
-      <c r="AL25" s="46"/>
-      <c r="AM25" s="46"/>
+      <c r="L25" s="49"/>
+      <c r="M25" s="49"/>
+      <c r="N25" s="49"/>
+      <c r="O25" s="49"/>
+      <c r="P25" s="49"/>
+      <c r="Q25" s="49"/>
+      <c r="R25" s="49"/>
+      <c r="S25" s="49"/>
+      <c r="T25" s="49"/>
+      <c r="U25" s="49"/>
+      <c r="V25" s="49"/>
+      <c r="W25" s="49"/>
+      <c r="X25" s="49"/>
+      <c r="Y25" s="49"/>
+      <c r="Z25" s="49"/>
+      <c r="AA25" s="49"/>
+      <c r="AB25" s="49"/>
+      <c r="AC25" s="49"/>
+      <c r="AD25" s="49"/>
+      <c r="AE25" s="49"/>
+      <c r="AF25" s="49"/>
+      <c r="AG25" s="49"/>
+      <c r="AH25" s="49"/>
+      <c r="AI25" s="49"/>
+      <c r="AJ25" s="49"/>
+      <c r="AK25" s="49"/>
+      <c r="AL25" s="49"/>
+      <c r="AM25" s="49"/>
       <c r="AN25" s="1"/>
       <c r="AO25" s="1"/>
       <c r="AP25" s="1"/>
@@ -5468,19 +5468,19 @@
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
-      <c r="U33" s="33" t="s">
+      <c r="U33" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="V33" s="34"/>
-      <c r="W33" s="34"/>
-      <c r="X33" s="34"/>
-      <c r="Y33" s="34"/>
-      <c r="Z33" s="34"/>
-      <c r="AA33" s="34"/>
-      <c r="AB33" s="34"/>
-      <c r="AC33" s="34"/>
-      <c r="AD33" s="34"/>
-      <c r="AE33" s="35"/>
+      <c r="V33" s="37"/>
+      <c r="W33" s="37"/>
+      <c r="X33" s="37"/>
+      <c r="Y33" s="37"/>
+      <c r="Z33" s="37"/>
+      <c r="AA33" s="37"/>
+      <c r="AB33" s="37"/>
+      <c r="AC33" s="37"/>
+      <c r="AD33" s="37"/>
+      <c r="AE33" s="38"/>
       <c r="AF33" s="1"/>
       <c r="AG33" s="1"/>
       <c r="AH33" s="1"/>
@@ -5522,17 +5522,17 @@
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
       <c r="T34" s="1"/>
-      <c r="U34" s="36"/>
-      <c r="V34" s="37"/>
-      <c r="W34" s="37"/>
-      <c r="X34" s="37"/>
-      <c r="Y34" s="37"/>
-      <c r="Z34" s="37"/>
-      <c r="AA34" s="37"/>
-      <c r="AB34" s="37"/>
-      <c r="AC34" s="37"/>
-      <c r="AD34" s="37"/>
-      <c r="AE34" s="38"/>
+      <c r="U34" s="39"/>
+      <c r="V34" s="40"/>
+      <c r="W34" s="40"/>
+      <c r="X34" s="40"/>
+      <c r="Y34" s="40"/>
+      <c r="Z34" s="40"/>
+      <c r="AA34" s="40"/>
+      <c r="AB34" s="40"/>
+      <c r="AC34" s="40"/>
+      <c r="AD34" s="40"/>
+      <c r="AE34" s="41"/>
       <c r="AF34" s="1"/>
       <c r="AG34" s="1"/>
       <c r="AH34" s="1"/>
@@ -5574,17 +5574,17 @@
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
       <c r="T35" s="1"/>
-      <c r="U35" s="36"/>
-      <c r="V35" s="37"/>
-      <c r="W35" s="37"/>
-      <c r="X35" s="37"/>
-      <c r="Y35" s="37"/>
-      <c r="Z35" s="37"/>
-      <c r="AA35" s="37"/>
-      <c r="AB35" s="37"/>
-      <c r="AC35" s="37"/>
-      <c r="AD35" s="37"/>
-      <c r="AE35" s="38"/>
+      <c r="U35" s="39"/>
+      <c r="V35" s="40"/>
+      <c r="W35" s="40"/>
+      <c r="X35" s="40"/>
+      <c r="Y35" s="40"/>
+      <c r="Z35" s="40"/>
+      <c r="AA35" s="40"/>
+      <c r="AB35" s="40"/>
+      <c r="AC35" s="40"/>
+      <c r="AD35" s="40"/>
+      <c r="AE35" s="41"/>
       <c r="AF35" s="1"/>
       <c r="AG35" s="1"/>
       <c r="AH35" s="1"/>
@@ -5626,17 +5626,17 @@
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
       <c r="T36" s="1"/>
-      <c r="U36" s="39"/>
-      <c r="V36" s="40"/>
-      <c r="W36" s="40"/>
-      <c r="X36" s="40"/>
-      <c r="Y36" s="40"/>
-      <c r="Z36" s="40"/>
-      <c r="AA36" s="40"/>
-      <c r="AB36" s="40"/>
-      <c r="AC36" s="40"/>
-      <c r="AD36" s="40"/>
-      <c r="AE36" s="41"/>
+      <c r="U36" s="42"/>
+      <c r="V36" s="43"/>
+      <c r="W36" s="43"/>
+      <c r="X36" s="43"/>
+      <c r="Y36" s="43"/>
+      <c r="Z36" s="43"/>
+      <c r="AA36" s="43"/>
+      <c r="AB36" s="43"/>
+      <c r="AC36" s="43"/>
+      <c r="AD36" s="43"/>
+      <c r="AE36" s="44"/>
       <c r="AF36" s="1"/>
       <c r="AG36" s="1"/>
       <c r="AH36" s="1"/>
@@ -5784,8 +5784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAFD2404-08A9-4D6B-860A-D0476E2ADAD6}">
   <dimension ref="B1:M445"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" zeroHeight="1" x14ac:dyDescent="0.3"/>
@@ -5793,12 +5793,16 @@
     <col min="1" max="16383" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.3"/>
+    <row r="1" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>95</v>
+      </c>
+    </row>
     <row r="2" spans="2:13" ht="26.25" x14ac:dyDescent="0.3">
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="50" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="47"/>
+      <c r="C2" s="50"/>
       <c r="D2" s="23"/>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
@@ -5816,20 +5820,20 @@
       </c>
     </row>
     <row r="4" spans="2:13" ht="26.25" x14ac:dyDescent="0.3">
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="47"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="50"/>
+      <c r="M4" s="50"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
@@ -5837,68 +5841,68 @@
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B6" s="119" t="s">
+      <c r="B6" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="119"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="53"/>
-      <c r="H6" s="53"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="53"/>
-      <c r="L6" s="53"/>
-      <c r="M6" s="53"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="60"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="60"/>
+      <c r="L6" s="60"/>
+      <c r="M6" s="60"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B7" s="120" t="s">
+      <c r="B7" s="51" t="s">
         <v>96</v>
       </c>
-      <c r="C7" s="121"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="49"/>
-      <c r="K7" s="49"/>
-      <c r="L7" s="49"/>
-      <c r="M7" s="50"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="55"/>
+      <c r="K7" s="55"/>
+      <c r="L7" s="55"/>
+      <c r="M7" s="56"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B8" s="119" t="s">
+      <c r="B8" s="59" t="s">
         <v>86</v>
       </c>
-      <c r="C8" s="119"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="53"/>
-      <c r="K8" s="53"/>
-      <c r="L8" s="53"/>
-      <c r="M8" s="53"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="60"/>
+      <c r="H8" s="60"/>
+      <c r="I8" s="60"/>
+      <c r="J8" s="60"/>
+      <c r="K8" s="60"/>
+      <c r="L8" s="60"/>
+      <c r="M8" s="60"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B9" s="119" t="s">
+      <c r="B9" s="59" t="s">
         <v>87</v>
       </c>
-      <c r="C9" s="119"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="53"/>
-      <c r="G9" s="53"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="53"/>
-      <c r="J9" s="53"/>
-      <c r="K9" s="53"/>
-      <c r="L9" s="53"/>
-      <c r="M9" s="53"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="60"/>
+      <c r="I9" s="60"/>
+      <c r="J9" s="60"/>
+      <c r="K9" s="60"/>
+      <c r="L9" s="60"/>
+      <c r="M9" s="60"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
@@ -5906,20 +5910,20 @@
       </c>
     </row>
     <row r="11" spans="2:13" ht="26.25" x14ac:dyDescent="0.3">
-      <c r="B11" s="47" t="s">
+      <c r="B11" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="C11" s="47"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="47"/>
-      <c r="H11" s="47"/>
-      <c r="I11" s="47"/>
-      <c r="J11" s="47"/>
-      <c r="K11" s="47"/>
-      <c r="L11" s="47"/>
-      <c r="M11" s="47"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="50"/>
+      <c r="M11" s="50"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
@@ -5948,12 +5952,12 @@
       </c>
     </row>
     <row r="16" spans="2:13" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="J16" s="51" t="s">
+      <c r="J16" s="57" t="s">
         <v>92</v>
       </c>
-      <c r="K16" s="52"/>
-      <c r="L16" s="52"/>
-      <c r="M16" s="52"/>
+      <c r="K16" s="58"/>
+      <c r="L16" s="58"/>
+      <c r="M16" s="58"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.3">
       <c r="J17" t="s">
@@ -5961,16 +5965,16 @@
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="J18" s="118" t="s">
+      <c r="J18" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="K18" s="118" t="s">
+      <c r="K18" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="L18" s="118" t="s">
+      <c r="L18" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="M18" s="118" t="s">
+      <c r="M18" s="25" t="s">
         <v>91</v>
       </c>
     </row>
@@ -6019,12 +6023,12 @@
       </c>
     </row>
     <row r="26" spans="2:13" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="J26" s="52" t="s">
+      <c r="J26" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="K26" s="52"/>
-      <c r="L26" s="52"/>
-      <c r="M26" s="52"/>
+      <c r="K26" s="58"/>
+      <c r="L26" s="58"/>
+      <c r="M26" s="58"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.3">
       <c r="J27" t="s">
@@ -6032,16 +6036,16 @@
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="J28" s="118" t="s">
+      <c r="J28" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="K28" s="118" t="s">
+      <c r="K28" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="L28" s="118" t="s">
+      <c r="L28" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="M28" s="118" t="s">
+      <c r="M28" s="25" t="s">
         <v>91</v>
       </c>
     </row>
@@ -6097,20 +6101,20 @@
       <c r="M32" s="18"/>
     </row>
     <row r="33" spans="2:13" ht="26.25" x14ac:dyDescent="0.3">
-      <c r="B33" s="47" t="s">
+      <c r="B33" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="C33" s="47"/>
-      <c r="D33" s="47"/>
-      <c r="E33" s="47"/>
-      <c r="F33" s="47"/>
-      <c r="G33" s="47"/>
-      <c r="H33" s="47"/>
-      <c r="I33" s="47"/>
-      <c r="J33" s="47"/>
-      <c r="K33" s="47"/>
-      <c r="L33" s="47"/>
-      <c r="M33" s="47"/>
+      <c r="C33" s="50"/>
+      <c r="D33" s="50"/>
+      <c r="E33" s="50"/>
+      <c r="F33" s="50"/>
+      <c r="G33" s="50"/>
+      <c r="H33" s="50"/>
+      <c r="I33" s="50"/>
+      <c r="J33" s="50"/>
+      <c r="K33" s="50"/>
+      <c r="L33" s="50"/>
+      <c r="M33" s="50"/>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
@@ -6118,24 +6122,24 @@
       </c>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B35" s="120" t="s">
+      <c r="B35" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C35" s="121"/>
-      <c r="D35" s="120" t="s">
+      <c r="C35" s="53"/>
+      <c r="D35" s="51" t="s">
         <v>94</v>
       </c>
-      <c r="E35" s="122"/>
-      <c r="F35" s="122"/>
-      <c r="G35" s="122"/>
-      <c r="H35" s="122"/>
-      <c r="I35" s="122"/>
-      <c r="J35" s="122"/>
-      <c r="K35" s="121"/>
-      <c r="L35" s="118" t="s">
+      <c r="E35" s="52"/>
+      <c r="F35" s="52"/>
+      <c r="G35" s="52"/>
+      <c r="H35" s="52"/>
+      <c r="I35" s="52"/>
+      <c r="J35" s="52"/>
+      <c r="K35" s="53"/>
+      <c r="L35" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="M35" s="118" t="s">
+      <c r="M35" s="25" t="s">
         <v>79</v>
       </c>
     </row>
@@ -17600,33 +17604,38 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B587F47-685F-4879-A76D-0E113D0E05A2}">
-  <dimension ref="B2:M2"/>
+  <dimension ref="B1:M2"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14.125" customWidth="1"/>
-    <col min="3" max="3" width="92.25" style="123" customWidth="1"/>
+    <col min="3" max="3" width="92.25" style="26" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>95</v>
+      </c>
+    </row>
     <row r="2" spans="2:13" ht="26.25" x14ac:dyDescent="0.3">
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="50" t="s">
         <v>102</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="117"/>
-      <c r="E2" s="117"/>
-      <c r="F2" s="117"/>
-      <c r="G2" s="117"/>
-      <c r="H2" s="117"/>
-      <c r="I2" s="117"/>
-      <c r="J2" s="117"/>
-      <c r="K2" s="117"/>
-      <c r="L2" s="117"/>
-      <c r="M2" s="117"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -17634,15 +17643,16 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5A6C62B-F631-4EF4-8E30-793E64FBA599}">
-  <dimension ref="B2:M4"/>
+  <dimension ref="B1:M4"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -17651,48 +17661,58 @@
     <col min="3" max="3" width="9" customWidth="1"/>
     <col min="4" max="4" width="60.625" customWidth="1"/>
     <col min="5" max="6" width="9" customWidth="1"/>
-    <col min="7" max="9" width="28.625" customWidth="1"/>
+    <col min="7" max="9" width="20.625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>95</v>
+      </c>
+    </row>
     <row r="2" spans="2:13" ht="26.25" x14ac:dyDescent="0.3">
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="50" t="s">
         <v>103</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="117"/>
-      <c r="K2" s="117"/>
-      <c r="L2" s="117"/>
-      <c r="M2" s="117"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B4" s="118" t="s">
+      <c r="B4" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="118" t="s">
+      <c r="C4" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="D4" s="118" t="s">
+      <c r="D4" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="118" t="s">
+      <c r="E4" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="118" t="s">
+      <c r="F4" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="G4" s="118" t="s">
+      <c r="G4" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="H4" s="118" t="s">
+      <c r="H4" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="I4" s="118" t="s">
+      <c r="I4" s="25" t="s">
         <v>108</v>
       </c>
     </row>
@@ -17724,14 +17744,14 @@
   <sheetData>
     <row r="1" spans="2:12" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:12" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -17813,157 +17833,157 @@
       <c r="J8" s="3"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B9" s="55" t="s">
+      <c r="B9" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="56"/>
-      <c r="D9" s="56" t="s">
+      <c r="C9" s="63"/>
+      <c r="D9" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="56"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="56"/>
-      <c r="H9" s="56"/>
-      <c r="I9" s="56"/>
-      <c r="J9" s="56"/>
-      <c r="K9" s="56" t="s">
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="63"/>
+      <c r="H9" s="63"/>
+      <c r="I9" s="63"/>
+      <c r="J9" s="63"/>
+      <c r="K9" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="L9" s="57"/>
+      <c r="L9" s="64"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B10" s="58" t="s">
+      <c r="B10" s="65" t="s">
         <v>76</v>
       </c>
-      <c r="C10" s="58"/>
-      <c r="D10" s="59" t="s">
+      <c r="C10" s="65"/>
+      <c r="D10" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="59"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="59"/>
-      <c r="J10" s="59"/>
-      <c r="K10" s="58">
+      <c r="E10" s="66"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="66"/>
+      <c r="I10" s="66"/>
+      <c r="J10" s="66"/>
+      <c r="K10" s="65">
         <v>1</v>
       </c>
-      <c r="L10" s="58"/>
+      <c r="L10" s="65"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B11" s="58"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="60" t="s">
+      <c r="B11" s="65"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="60"/>
-      <c r="J11" s="60"/>
-      <c r="K11" s="58"/>
-      <c r="L11" s="58"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="67"/>
+      <c r="J11" s="67"/>
+      <c r="K11" s="65"/>
+      <c r="L11" s="65"/>
     </row>
     <row r="12" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="61" t="s">
+      <c r="B12" s="68" t="s">
         <v>80</v>
       </c>
-      <c r="C12" s="62"/>
-      <c r="D12" s="65" t="s">
+      <c r="C12" s="69"/>
+      <c r="D12" s="72" t="s">
         <v>81</v>
       </c>
-      <c r="E12" s="66"/>
-      <c r="F12" s="66"/>
-      <c r="G12" s="66"/>
-      <c r="H12" s="66"/>
-      <c r="I12" s="66"/>
-      <c r="J12" s="67"/>
-      <c r="K12" s="61">
+      <c r="E12" s="73"/>
+      <c r="F12" s="73"/>
+      <c r="G12" s="73"/>
+      <c r="H12" s="73"/>
+      <c r="I12" s="73"/>
+      <c r="J12" s="74"/>
+      <c r="K12" s="68">
         <v>0.5</v>
       </c>
-      <c r="L12" s="62"/>
+      <c r="L12" s="69"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B13" s="63"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="68"/>
-      <c r="E13" s="69"/>
-      <c r="F13" s="69"/>
-      <c r="G13" s="69"/>
-      <c r="H13" s="69"/>
-      <c r="I13" s="69"/>
-      <c r="J13" s="70"/>
-      <c r="K13" s="63"/>
-      <c r="L13" s="64"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="71"/>
+      <c r="D13" s="75"/>
+      <c r="E13" s="76"/>
+      <c r="F13" s="76"/>
+      <c r="G13" s="76"/>
+      <c r="H13" s="76"/>
+      <c r="I13" s="76"/>
+      <c r="J13" s="77"/>
+      <c r="K13" s="70"/>
+      <c r="L13" s="71"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="58" t="s">
+      <c r="B14" s="65" t="s">
         <v>77</v>
       </c>
-      <c r="C14" s="58"/>
-      <c r="D14" s="59" t="s">
+      <c r="C14" s="65"/>
+      <c r="D14" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="59"/>
-      <c r="F14" s="59"/>
-      <c r="G14" s="59"/>
-      <c r="H14" s="59"/>
-      <c r="I14" s="59"/>
-      <c r="J14" s="59"/>
-      <c r="K14" s="58">
+      <c r="E14" s="66"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="66"/>
+      <c r="H14" s="66"/>
+      <c r="I14" s="66"/>
+      <c r="J14" s="66"/>
+      <c r="K14" s="65">
         <v>0</v>
       </c>
-      <c r="L14" s="58"/>
+      <c r="L14" s="65"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B15" s="58"/>
-      <c r="C15" s="58"/>
-      <c r="D15" s="60" t="s">
+      <c r="B15" s="65"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="60"/>
-      <c r="F15" s="60"/>
-      <c r="G15" s="60"/>
-      <c r="H15" s="60"/>
-      <c r="I15" s="60"/>
-      <c r="J15" s="60"/>
-      <c r="K15" s="58"/>
-      <c r="L15" s="58"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="67"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="67"/>
+      <c r="I15" s="67"/>
+      <c r="J15" s="67"/>
+      <c r="K15" s="65"/>
+      <c r="L15" s="65"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B16" s="58" t="s">
+      <c r="B16" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="58"/>
-      <c r="D16" s="59" t="s">
+      <c r="C16" s="65"/>
+      <c r="D16" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="59"/>
-      <c r="F16" s="59"/>
-      <c r="G16" s="59"/>
-      <c r="H16" s="59"/>
-      <c r="I16" s="59"/>
-      <c r="J16" s="59"/>
-      <c r="K16" s="58" t="s">
+      <c r="E16" s="66"/>
+      <c r="F16" s="66"/>
+      <c r="G16" s="66"/>
+      <c r="H16" s="66"/>
+      <c r="I16" s="66"/>
+      <c r="J16" s="66"/>
+      <c r="K16" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="L16" s="58"/>
+      <c r="L16" s="65"/>
     </row>
     <row r="17" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="71"/>
-      <c r="C17" s="71"/>
-      <c r="D17" s="72" t="s">
+      <c r="B17" s="78"/>
+      <c r="C17" s="78"/>
+      <c r="D17" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="72"/>
-      <c r="F17" s="72"/>
-      <c r="G17" s="72"/>
-      <c r="H17" s="72"/>
-      <c r="I17" s="72"/>
-      <c r="J17" s="72"/>
-      <c r="K17" s="71"/>
-      <c r="L17" s="71"/>
+      <c r="E17" s="79"/>
+      <c r="F17" s="79"/>
+      <c r="G17" s="79"/>
+      <c r="H17" s="79"/>
+      <c r="I17" s="79"/>
+      <c r="J17" s="79"/>
+      <c r="K17" s="78"/>
+      <c r="L17" s="78"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" s="6"/>
@@ -18016,200 +18036,200 @@
       <c r="J21" s="3"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B22" s="73" t="s">
+      <c r="B22" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="74"/>
-      <c r="D22" s="75" t="s">
+      <c r="C22" s="81"/>
+      <c r="D22" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="E22" s="76"/>
-      <c r="F22" s="76"/>
-      <c r="G22" s="76"/>
-      <c r="H22" s="76"/>
-      <c r="I22" s="76"/>
-      <c r="J22" s="74"/>
-      <c r="K22" s="77" t="s">
+      <c r="E22" s="83"/>
+      <c r="F22" s="83"/>
+      <c r="G22" s="83"/>
+      <c r="H22" s="83"/>
+      <c r="I22" s="83"/>
+      <c r="J22" s="81"/>
+      <c r="K22" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="L22" s="78"/>
+      <c r="L22" s="85"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B23" s="79" t="s">
+      <c r="B23" s="86" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="79"/>
-      <c r="D23" s="80" t="s">
+      <c r="C23" s="86"/>
+      <c r="D23" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="E23" s="81"/>
-      <c r="F23" s="81"/>
-      <c r="G23" s="81"/>
-      <c r="H23" s="81"/>
-      <c r="I23" s="81"/>
-      <c r="J23" s="82"/>
-      <c r="K23" s="83" t="s">
+      <c r="E23" s="88"/>
+      <c r="F23" s="88"/>
+      <c r="G23" s="88"/>
+      <c r="H23" s="88"/>
+      <c r="I23" s="88"/>
+      <c r="J23" s="89"/>
+      <c r="K23" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="L23" s="84"/>
+      <c r="L23" s="91"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B24" s="79"/>
-      <c r="C24" s="79"/>
-      <c r="D24" s="89" t="s">
+      <c r="B24" s="86"/>
+      <c r="C24" s="86"/>
+      <c r="D24" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="90"/>
-      <c r="F24" s="90"/>
-      <c r="G24" s="90"/>
-      <c r="H24" s="90"/>
-      <c r="I24" s="90"/>
-      <c r="J24" s="91"/>
-      <c r="K24" s="85"/>
-      <c r="L24" s="86"/>
+      <c r="E24" s="97"/>
+      <c r="F24" s="97"/>
+      <c r="G24" s="97"/>
+      <c r="H24" s="97"/>
+      <c r="I24" s="97"/>
+      <c r="J24" s="98"/>
+      <c r="K24" s="92"/>
+      <c r="L24" s="93"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B25" s="79"/>
-      <c r="C25" s="79"/>
-      <c r="D25" s="89" t="s">
+      <c r="B25" s="86"/>
+      <c r="C25" s="86"/>
+      <c r="D25" s="96" t="s">
         <v>30</v>
       </c>
-      <c r="E25" s="90"/>
-      <c r="F25" s="90"/>
-      <c r="G25" s="90"/>
-      <c r="H25" s="90"/>
-      <c r="I25" s="90"/>
-      <c r="J25" s="91"/>
-      <c r="K25" s="85"/>
-      <c r="L25" s="86"/>
+      <c r="E25" s="97"/>
+      <c r="F25" s="97"/>
+      <c r="G25" s="97"/>
+      <c r="H25" s="97"/>
+      <c r="I25" s="97"/>
+      <c r="J25" s="98"/>
+      <c r="K25" s="92"/>
+      <c r="L25" s="93"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B26" s="79"/>
-      <c r="C26" s="79"/>
-      <c r="D26" s="92" t="s">
+      <c r="B26" s="86"/>
+      <c r="C26" s="86"/>
+      <c r="D26" s="99" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="93"/>
-      <c r="F26" s="93"/>
-      <c r="G26" s="93"/>
-      <c r="H26" s="93"/>
-      <c r="I26" s="93"/>
-      <c r="J26" s="94"/>
-      <c r="K26" s="87"/>
-      <c r="L26" s="88"/>
+      <c r="E26" s="100"/>
+      <c r="F26" s="100"/>
+      <c r="G26" s="100"/>
+      <c r="H26" s="100"/>
+      <c r="I26" s="100"/>
+      <c r="J26" s="101"/>
+      <c r="K26" s="94"/>
+      <c r="L26" s="95"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B27" s="79" t="s">
+      <c r="B27" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="95"/>
-      <c r="D27" s="89" t="s">
+      <c r="C27" s="102"/>
+      <c r="D27" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="E27" s="90"/>
-      <c r="F27" s="90"/>
-      <c r="G27" s="90"/>
-      <c r="H27" s="90"/>
-      <c r="I27" s="90"/>
-      <c r="J27" s="91"/>
-      <c r="K27" s="83" t="s">
+      <c r="E27" s="97"/>
+      <c r="F27" s="97"/>
+      <c r="G27" s="97"/>
+      <c r="H27" s="97"/>
+      <c r="I27" s="97"/>
+      <c r="J27" s="98"/>
+      <c r="K27" s="90" t="s">
         <v>34</v>
       </c>
-      <c r="L27" s="84"/>
+      <c r="L27" s="91"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B28" s="95"/>
-      <c r="C28" s="95"/>
-      <c r="D28" s="89" t="s">
+      <c r="B28" s="102"/>
+      <c r="C28" s="102"/>
+      <c r="D28" s="96" t="s">
         <v>35</v>
       </c>
-      <c r="E28" s="90"/>
-      <c r="F28" s="90"/>
-      <c r="G28" s="90"/>
-      <c r="H28" s="90"/>
-      <c r="I28" s="90"/>
-      <c r="J28" s="91"/>
-      <c r="K28" s="85"/>
-      <c r="L28" s="86"/>
+      <c r="E28" s="97"/>
+      <c r="F28" s="97"/>
+      <c r="G28" s="97"/>
+      <c r="H28" s="97"/>
+      <c r="I28" s="97"/>
+      <c r="J28" s="98"/>
+      <c r="K28" s="92"/>
+      <c r="L28" s="93"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B29" s="95"/>
-      <c r="C29" s="95"/>
-      <c r="D29" s="92" t="s">
+      <c r="B29" s="102"/>
+      <c r="C29" s="102"/>
+      <c r="D29" s="99" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="93"/>
-      <c r="F29" s="93"/>
-      <c r="G29" s="93"/>
-      <c r="H29" s="93"/>
-      <c r="I29" s="93"/>
-      <c r="J29" s="94"/>
-      <c r="K29" s="87"/>
-      <c r="L29" s="88"/>
+      <c r="E29" s="100"/>
+      <c r="F29" s="100"/>
+      <c r="G29" s="100"/>
+      <c r="H29" s="100"/>
+      <c r="I29" s="100"/>
+      <c r="J29" s="101"/>
+      <c r="K29" s="94"/>
+      <c r="L29" s="95"/>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B30" s="79" t="s">
+      <c r="B30" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="95"/>
-      <c r="D30" s="80" t="s">
+      <c r="C30" s="102"/>
+      <c r="D30" s="87" t="s">
         <v>38</v>
       </c>
-      <c r="E30" s="81"/>
-      <c r="F30" s="81"/>
-      <c r="G30" s="81"/>
-      <c r="H30" s="81"/>
-      <c r="I30" s="81"/>
-      <c r="J30" s="82"/>
-      <c r="K30" s="83" t="s">
+      <c r="E30" s="88"/>
+      <c r="F30" s="88"/>
+      <c r="G30" s="88"/>
+      <c r="H30" s="88"/>
+      <c r="I30" s="88"/>
+      <c r="J30" s="89"/>
+      <c r="K30" s="90" t="s">
         <v>39</v>
       </c>
-      <c r="L30" s="84"/>
+      <c r="L30" s="91"/>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B31" s="95"/>
-      <c r="C31" s="95"/>
-      <c r="D31" s="89" t="s">
+      <c r="B31" s="102"/>
+      <c r="C31" s="102"/>
+      <c r="D31" s="96" t="s">
         <v>40</v>
       </c>
-      <c r="E31" s="90"/>
-      <c r="F31" s="90"/>
-      <c r="G31" s="90"/>
-      <c r="H31" s="90"/>
-      <c r="I31" s="90"/>
-      <c r="J31" s="91"/>
-      <c r="K31" s="85"/>
-      <c r="L31" s="86"/>
+      <c r="E31" s="97"/>
+      <c r="F31" s="97"/>
+      <c r="G31" s="97"/>
+      <c r="H31" s="97"/>
+      <c r="I31" s="97"/>
+      <c r="J31" s="98"/>
+      <c r="K31" s="92"/>
+      <c r="L31" s="93"/>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B32" s="95"/>
-      <c r="C32" s="95"/>
-      <c r="D32" s="89" t="s">
+      <c r="B32" s="102"/>
+      <c r="C32" s="102"/>
+      <c r="D32" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="E32" s="90"/>
-      <c r="F32" s="90"/>
-      <c r="G32" s="90"/>
-      <c r="H32" s="90"/>
-      <c r="I32" s="90"/>
-      <c r="J32" s="91"/>
-      <c r="K32" s="85"/>
-      <c r="L32" s="86"/>
+      <c r="E32" s="97"/>
+      <c r="F32" s="97"/>
+      <c r="G32" s="97"/>
+      <c r="H32" s="97"/>
+      <c r="I32" s="97"/>
+      <c r="J32" s="98"/>
+      <c r="K32" s="92"/>
+      <c r="L32" s="93"/>
     </row>
     <row r="33" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="96"/>
-      <c r="C33" s="96"/>
-      <c r="D33" s="99" t="s">
+      <c r="B33" s="103"/>
+      <c r="C33" s="103"/>
+      <c r="D33" s="106" t="s">
         <v>42</v>
       </c>
-      <c r="E33" s="100"/>
-      <c r="F33" s="100"/>
-      <c r="G33" s="100"/>
-      <c r="H33" s="100"/>
-      <c r="I33" s="100"/>
-      <c r="J33" s="101"/>
-      <c r="K33" s="97"/>
-      <c r="L33" s="98"/>
+      <c r="E33" s="107"/>
+      <c r="F33" s="107"/>
+      <c r="G33" s="107"/>
+      <c r="H33" s="107"/>
+      <c r="I33" s="107"/>
+      <c r="J33" s="108"/>
+      <c r="K33" s="104"/>
+      <c r="L33" s="105"/>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B34" s="10"/>
@@ -18286,38 +18306,38 @@
       <c r="J39" s="3"/>
     </row>
     <row r="40" spans="2:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="108" t="s">
+      <c r="B40" s="115" t="s">
         <v>47</v>
       </c>
-      <c r="C40" s="109"/>
-      <c r="D40" s="109"/>
-      <c r="E40" s="111" t="s">
+      <c r="C40" s="116"/>
+      <c r="D40" s="116"/>
+      <c r="E40" s="118" t="s">
         <v>98</v>
       </c>
-      <c r="F40" s="111"/>
-      <c r="G40" s="111"/>
-      <c r="H40" s="111"/>
-      <c r="I40" s="111"/>
-      <c r="J40" s="111"/>
-      <c r="K40" s="81" t="s">
+      <c r="F40" s="118"/>
+      <c r="G40" s="118"/>
+      <c r="H40" s="118"/>
+      <c r="I40" s="118"/>
+      <c r="J40" s="118"/>
+      <c r="K40" s="88" t="s">
         <v>48</v>
       </c>
-      <c r="L40" s="82"/>
+      <c r="L40" s="89"/>
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B41" s="110"/>
-      <c r="C41" s="102"/>
-      <c r="D41" s="102"/>
-      <c r="E41" s="102" t="s">
+      <c r="B41" s="117"/>
+      <c r="C41" s="109"/>
+      <c r="D41" s="109"/>
+      <c r="E41" s="109" t="s">
         <v>99</v>
       </c>
-      <c r="F41" s="102"/>
-      <c r="G41" s="102"/>
-      <c r="H41" s="102"/>
-      <c r="I41" s="102"/>
-      <c r="J41" s="102"/>
-      <c r="K41" s="93"/>
-      <c r="L41" s="94"/>
+      <c r="F41" s="109"/>
+      <c r="G41" s="109"/>
+      <c r="H41" s="109"/>
+      <c r="I41" s="109"/>
+      <c r="J41" s="109"/>
+      <c r="K41" s="100"/>
+      <c r="L41" s="101"/>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B42" s="3"/>
@@ -18370,193 +18390,193 @@
       <c r="J45" s="3"/>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B46" s="73" t="s">
+      <c r="B46" s="80" t="s">
         <v>52</v>
       </c>
-      <c r="C46" s="74"/>
-      <c r="D46" s="56" t="s">
+      <c r="C46" s="81"/>
+      <c r="D46" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="E46" s="56"/>
-      <c r="F46" s="75" t="s">
+      <c r="E46" s="63"/>
+      <c r="F46" s="82" t="s">
         <v>54</v>
       </c>
-      <c r="G46" s="76"/>
-      <c r="H46" s="76"/>
-      <c r="I46" s="76"/>
-      <c r="J46" s="76"/>
-      <c r="K46" s="76"/>
-      <c r="L46" s="76"/>
+      <c r="G46" s="83"/>
+      <c r="H46" s="83"/>
+      <c r="I46" s="83"/>
+      <c r="J46" s="83"/>
+      <c r="K46" s="83"/>
+      <c r="L46" s="83"/>
     </row>
     <row r="47" spans="2:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="103" t="s">
+      <c r="B47" s="110" t="s">
         <v>55</v>
       </c>
-      <c r="C47" s="103"/>
-      <c r="D47" s="104" t="s">
+      <c r="C47" s="110"/>
+      <c r="D47" s="111" t="s">
         <v>56</v>
       </c>
-      <c r="E47" s="104"/>
-      <c r="F47" s="105" t="s">
+      <c r="E47" s="111"/>
+      <c r="F47" s="112" t="s">
         <v>57</v>
       </c>
-      <c r="G47" s="105"/>
-      <c r="H47" s="105"/>
-      <c r="I47" s="105"/>
-      <c r="J47" s="105"/>
-      <c r="K47" s="105"/>
-      <c r="L47" s="105"/>
+      <c r="G47" s="112"/>
+      <c r="H47" s="112"/>
+      <c r="I47" s="112"/>
+      <c r="J47" s="112"/>
+      <c r="K47" s="112"/>
+      <c r="L47" s="112"/>
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B48" s="103"/>
-      <c r="C48" s="103"/>
-      <c r="D48" s="104"/>
-      <c r="E48" s="104"/>
-      <c r="F48" s="106" t="s">
+      <c r="B48" s="110"/>
+      <c r="C48" s="110"/>
+      <c r="D48" s="111"/>
+      <c r="E48" s="111"/>
+      <c r="F48" s="113" t="s">
         <v>58</v>
       </c>
-      <c r="G48" s="106"/>
-      <c r="H48" s="106"/>
-      <c r="I48" s="106"/>
-      <c r="J48" s="106"/>
-      <c r="K48" s="106"/>
-      <c r="L48" s="107"/>
+      <c r="G48" s="113"/>
+      <c r="H48" s="113"/>
+      <c r="I48" s="113"/>
+      <c r="J48" s="113"/>
+      <c r="K48" s="113"/>
+      <c r="L48" s="114"/>
     </row>
     <row r="49" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B49" s="103" t="s">
+      <c r="B49" s="110" t="s">
         <v>59</v>
       </c>
-      <c r="C49" s="103"/>
-      <c r="D49" s="104" t="s">
+      <c r="C49" s="110"/>
+      <c r="D49" s="111" t="s">
         <v>60</v>
       </c>
-      <c r="E49" s="104"/>
-      <c r="F49" s="105" t="s">
+      <c r="E49" s="111"/>
+      <c r="F49" s="112" t="s">
         <v>57</v>
       </c>
-      <c r="G49" s="105"/>
-      <c r="H49" s="105"/>
-      <c r="I49" s="105"/>
-      <c r="J49" s="105"/>
-      <c r="K49" s="105"/>
-      <c r="L49" s="112"/>
+      <c r="G49" s="112"/>
+      <c r="H49" s="112"/>
+      <c r="I49" s="112"/>
+      <c r="J49" s="112"/>
+      <c r="K49" s="112"/>
+      <c r="L49" s="119"/>
     </row>
     <row r="50" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B50" s="103"/>
-      <c r="C50" s="103"/>
-      <c r="D50" s="104"/>
-      <c r="E50" s="104"/>
-      <c r="F50" s="106" t="s">
+      <c r="B50" s="110"/>
+      <c r="C50" s="110"/>
+      <c r="D50" s="111"/>
+      <c r="E50" s="111"/>
+      <c r="F50" s="113" t="s">
         <v>61</v>
       </c>
-      <c r="G50" s="106"/>
-      <c r="H50" s="106"/>
-      <c r="I50" s="106"/>
-      <c r="J50" s="106"/>
-      <c r="K50" s="106"/>
-      <c r="L50" s="107"/>
+      <c r="G50" s="113"/>
+      <c r="H50" s="113"/>
+      <c r="I50" s="113"/>
+      <c r="J50" s="113"/>
+      <c r="K50" s="113"/>
+      <c r="L50" s="114"/>
     </row>
     <row r="51" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B51" s="103" t="s">
+      <c r="B51" s="110" t="s">
         <v>62</v>
       </c>
-      <c r="C51" s="103"/>
-      <c r="D51" s="104" t="s">
+      <c r="C51" s="110"/>
+      <c r="D51" s="111" t="s">
         <v>63</v>
       </c>
-      <c r="E51" s="104"/>
-      <c r="F51" s="105" t="s">
+      <c r="E51" s="111"/>
+      <c r="F51" s="112" t="s">
         <v>64</v>
       </c>
-      <c r="G51" s="105"/>
-      <c r="H51" s="105"/>
-      <c r="I51" s="105"/>
-      <c r="J51" s="105"/>
-      <c r="K51" s="105"/>
-      <c r="L51" s="112"/>
+      <c r="G51" s="112"/>
+      <c r="H51" s="112"/>
+      <c r="I51" s="112"/>
+      <c r="J51" s="112"/>
+      <c r="K51" s="112"/>
+      <c r="L51" s="119"/>
     </row>
     <row r="52" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B52" s="103"/>
-      <c r="C52" s="103"/>
-      <c r="D52" s="104"/>
-      <c r="E52" s="104"/>
-      <c r="F52" s="106" t="s">
+      <c r="B52" s="110"/>
+      <c r="C52" s="110"/>
+      <c r="D52" s="111"/>
+      <c r="E52" s="111"/>
+      <c r="F52" s="113" t="s">
         <v>65</v>
       </c>
-      <c r="G52" s="106"/>
-      <c r="H52" s="106"/>
-      <c r="I52" s="106"/>
-      <c r="J52" s="106"/>
-      <c r="K52" s="106"/>
-      <c r="L52" s="107"/>
+      <c r="G52" s="113"/>
+      <c r="H52" s="113"/>
+      <c r="I52" s="113"/>
+      <c r="J52" s="113"/>
+      <c r="K52" s="113"/>
+      <c r="L52" s="114"/>
     </row>
     <row r="53" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B53" s="103" t="s">
+      <c r="B53" s="110" t="s">
         <v>66</v>
       </c>
-      <c r="C53" s="103"/>
-      <c r="D53" s="104" t="s">
+      <c r="C53" s="110"/>
+      <c r="D53" s="111" t="s">
         <v>67</v>
       </c>
-      <c r="E53" s="104"/>
-      <c r="F53" s="105" t="s">
+      <c r="E53" s="111"/>
+      <c r="F53" s="112" t="s">
         <v>68</v>
       </c>
-      <c r="G53" s="105"/>
-      <c r="H53" s="105"/>
-      <c r="I53" s="105"/>
-      <c r="J53" s="105"/>
-      <c r="K53" s="105"/>
-      <c r="L53" s="112"/>
+      <c r="G53" s="112"/>
+      <c r="H53" s="112"/>
+      <c r="I53" s="112"/>
+      <c r="J53" s="112"/>
+      <c r="K53" s="112"/>
+      <c r="L53" s="119"/>
     </row>
     <row r="54" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B54" s="103"/>
-      <c r="C54" s="103"/>
-      <c r="D54" s="104"/>
-      <c r="E54" s="104"/>
-      <c r="F54" s="106" t="s">
+      <c r="B54" s="110"/>
+      <c r="C54" s="110"/>
+      <c r="D54" s="111"/>
+      <c r="E54" s="111"/>
+      <c r="F54" s="113" t="s">
         <v>69</v>
       </c>
-      <c r="G54" s="106"/>
-      <c r="H54" s="106"/>
-      <c r="I54" s="106"/>
-      <c r="J54" s="106"/>
-      <c r="K54" s="106"/>
-      <c r="L54" s="107"/>
+      <c r="G54" s="113"/>
+      <c r="H54" s="113"/>
+      <c r="I54" s="113"/>
+      <c r="J54" s="113"/>
+      <c r="K54" s="113"/>
+      <c r="L54" s="114"/>
     </row>
     <row r="55" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B55" s="103" t="s">
+      <c r="B55" s="110" t="s">
         <v>70</v>
       </c>
-      <c r="C55" s="103"/>
-      <c r="D55" s="104" t="s">
+      <c r="C55" s="110"/>
+      <c r="D55" s="111" t="s">
         <v>71</v>
       </c>
-      <c r="E55" s="104"/>
-      <c r="F55" s="105" t="s">
+      <c r="E55" s="111"/>
+      <c r="F55" s="112" t="s">
         <v>72</v>
       </c>
-      <c r="G55" s="105"/>
-      <c r="H55" s="105"/>
-      <c r="I55" s="105"/>
-      <c r="J55" s="105"/>
-      <c r="K55" s="105"/>
-      <c r="L55" s="112"/>
+      <c r="G55" s="112"/>
+      <c r="H55" s="112"/>
+      <c r="I55" s="112"/>
+      <c r="J55" s="112"/>
+      <c r="K55" s="112"/>
+      <c r="L55" s="119"/>
     </row>
     <row r="56" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B56" s="113"/>
-      <c r="C56" s="113"/>
-      <c r="D56" s="114"/>
-      <c r="E56" s="114"/>
-      <c r="F56" s="115" t="s">
+      <c r="B56" s="120"/>
+      <c r="C56" s="120"/>
+      <c r="D56" s="121"/>
+      <c r="E56" s="121"/>
+      <c r="F56" s="122" t="s">
         <v>73</v>
       </c>
-      <c r="G56" s="115"/>
-      <c r="H56" s="115"/>
-      <c r="I56" s="115"/>
-      <c r="J56" s="115"/>
-      <c r="K56" s="115"/>
-      <c r="L56" s="116"/>
+      <c r="G56" s="122"/>
+      <c r="H56" s="122"/>
+      <c r="I56" s="122"/>
+      <c r="J56" s="122"/>
+      <c r="K56" s="122"/>
+      <c r="L56" s="123"/>
     </row>
     <row r="57" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B57" s="14"/>

</xml_diff>